<commit_message>
Product name updated to rapise
</commit_message>
<xml_diff>
--- a/tools/KnowledgeBase2RapiseDoc/Main.rvl.xlsx
+++ b/tools/KnowledgeBase2RapiseDoc/Main.rvl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="442" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="443" uniqueCount="85">
   <si>
     <t>Flow</t>
   </si>
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H2" s="16"/>
     </row>

</xml_diff>